<commit_message>
created rvl file for creating doctor
</commit_message>
<xml_diff>
--- a/RapiseTestSamples/Sub_Test_1/Scenario_CreateDoctor200/Main.rvl.xlsx
+++ b/RapiseTestSamples/Sub_Test_1/Scenario_CreateDoctor200/Main.rvl.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="117">
   <si>
     <t>Flow</t>
   </si>
@@ -329,6 +329,42 @@
   </si>
   <si>
     <t>And check for id</t>
+  </si>
+  <si>
+    <t>590036950348</t>
+  </si>
+  <si>
+    <t>605045336809</t>
+  </si>
+  <si>
+    <t>605044336809</t>
+  </si>
+  <si>
+    <t>599036950348</t>
+  </si>
+  <si>
+    <t>599036900348</t>
+  </si>
+  <si>
+    <t>605040336809</t>
+  </si>
+  <si>
+    <t>605040336009</t>
+  </si>
+  <si>
+    <t>599036900308</t>
+  </si>
+  <si>
+    <t>999036900308</t>
+  </si>
+  <si>
+    <t>905040336009</t>
+  </si>
+  <si>
+    <t>998036900308</t>
+  </si>
+  <si>
+    <t>900040336009</t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1684,7 @@
         <v>63</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
         <v>65</v>
@@ -1666,7 +1702,7 @@
         <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
       <c r="F5" t="s">
         <v>70</v>
@@ -1707,7 +1743,7 @@
         <v>11</v>
       </c>
       <c r="G9" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
@@ -1737,7 +1773,7 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
@@ -1767,7 +1803,7 @@
         <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
@@ -2196,7 +2232,7 @@
         <v>11</v>
       </c>
       <c r="G51" t="s">
-        <v>69</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52">
@@ -2865,7 +2901,7 @@
         <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18">
@@ -2932,7 +2968,7 @@
         <v>40</v>
       </c>
       <c r="G23" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24">

</xml_diff>